<commit_message>
Adding Lidar for purchase to form
</commit_message>
<xml_diff>
--- a/Ursaworks Inventory & Purchase.xlsx
+++ b/Ursaworks Inventory & Purchase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluya\Documents\reimbursement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluya\Documents\GitHub\Ursaworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C80152-125D-425F-9292-598F6ACE81B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3874BCE1-87E2-4F8C-9C88-293448273571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="583">
   <si>
     <t>FINANCIAL REPORT</t>
   </si>
@@ -2216,6 +2216,15 @@
   </si>
   <si>
     <t>T-Slot Framing Bar: 20 mm x 20 mm x 10000mm</t>
+  </si>
+  <si>
+    <t>Sentry</t>
+  </si>
+  <si>
+    <t>Lidar</t>
+  </si>
+  <si>
+    <t>Amazon.com: WayPonDEV FHL-LD19 360 Degree 2D Lidar Distance Sensor Kit, 10Hz Scan Rate and 12m Distance Lidar Scanner Module for Smart Obstacle/Robot/Maker Education Indoor/Outdoor : Industrial &amp; Scientific</t>
   </si>
 </sst>
 </file>
@@ -6417,7 +6426,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B38" sqref="B38:B39"/>
+      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -9698,7 +9707,7 @@
       <c r="W96" s="17"/>
       <c r="X96" s="1"/>
     </row>
-    <row r="97" spans="8:24" ht="15.75" customHeight="1">
+    <row r="97" spans="1:24" ht="15.75" customHeight="1">
       <c r="H97" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9712,7 +9721,7 @@
       <c r="W97" s="17"/>
       <c r="X97" s="1"/>
     </row>
-    <row r="98" spans="8:24" ht="15.75" customHeight="1">
+    <row r="98" spans="1:24" ht="15.75" customHeight="1">
       <c r="H98" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9726,7 +9735,7 @@
       <c r="W98" s="17"/>
       <c r="X98" s="1"/>
     </row>
-    <row r="99" spans="8:24" ht="15.75" customHeight="1">
+    <row r="99" spans="1:24" ht="15.75" customHeight="1">
       <c r="H99" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9740,7 +9749,10 @@
       <c r="W99" s="17"/>
       <c r="X99" s="1"/>
     </row>
-    <row r="100" spans="8:24" ht="15.75" customHeight="1">
+    <row r="100" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A100" t="s">
+        <v>580</v>
+      </c>
       <c r="H100" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9754,7 +9766,13 @@
       <c r="W100" s="17"/>
       <c r="X100" s="1"/>
     </row>
-    <row r="101" spans="8:24" ht="15.75" customHeight="1">
+    <row r="101" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A101" t="s">
+        <v>581</v>
+      </c>
+      <c r="E101" s="116" t="s">
+        <v>582</v>
+      </c>
       <c r="H101" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9768,7 +9786,7 @@
       <c r="W101" s="17"/>
       <c r="X101" s="1"/>
     </row>
-    <row r="102" spans="8:24" ht="15.75" customHeight="1">
+    <row r="102" spans="1:24" ht="15.75" customHeight="1">
       <c r="H102" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9782,7 +9800,7 @@
       <c r="W102" s="17"/>
       <c r="X102" s="1"/>
     </row>
-    <row r="103" spans="8:24" ht="15.75" customHeight="1">
+    <row r="103" spans="1:24" ht="15.75" customHeight="1">
       <c r="H103" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9796,7 +9814,7 @@
       <c r="W103" s="17"/>
       <c r="X103" s="1"/>
     </row>
-    <row r="104" spans="8:24" ht="15.75" customHeight="1">
+    <row r="104" spans="1:24" ht="15.75" customHeight="1">
       <c r="M104" s="122"/>
       <c r="N104" s="1"/>
       <c r="O104" s="24"/>
@@ -9806,7 +9824,7 @@
       <c r="W104" s="17"/>
       <c r="X104" s="1"/>
     </row>
-    <row r="105" spans="8:24" ht="15.75" customHeight="1">
+    <row r="105" spans="1:24" ht="15.75" customHeight="1">
       <c r="M105" s="122"/>
       <c r="N105" s="1"/>
       <c r="O105" s="24"/>
@@ -9816,7 +9834,7 @@
       <c r="W105" s="17"/>
       <c r="X105" s="1"/>
     </row>
-    <row r="106" spans="8:24" ht="15.75" customHeight="1">
+    <row r="106" spans="1:24" ht="15.75" customHeight="1">
       <c r="M106" s="122"/>
       <c r="N106" s="1"/>
       <c r="O106" s="24"/>
@@ -9826,7 +9844,7 @@
       <c r="W106" s="17"/>
       <c r="X106" s="1"/>
     </row>
-    <row r="107" spans="8:24" ht="15.75" customHeight="1">
+    <row r="107" spans="1:24" ht="15.75" customHeight="1">
       <c r="M107" s="122"/>
       <c r="N107" s="1"/>
       <c r="O107" s="24"/>
@@ -9836,7 +9854,7 @@
       <c r="W107" s="17"/>
       <c r="X107" s="1"/>
     </row>
-    <row r="108" spans="8:24" ht="15.75" customHeight="1">
+    <row r="108" spans="1:24" ht="15.75" customHeight="1">
       <c r="M108" s="122"/>
       <c r="N108" s="1"/>
       <c r="O108" s="24"/>
@@ -9847,7 +9865,7 @@
       <c r="W108" s="17"/>
       <c r="X108" s="1"/>
     </row>
-    <row r="109" spans="8:24" ht="15.75" customHeight="1">
+    <row r="109" spans="1:24" ht="15.75" customHeight="1">
       <c r="M109" s="122"/>
       <c r="N109" s="1"/>
       <c r="O109" s="24"/>
@@ -9858,7 +9876,7 @@
       <c r="W109" s="17"/>
       <c r="X109" s="1"/>
     </row>
-    <row r="110" spans="8:24" ht="15.75" customHeight="1">
+    <row r="110" spans="1:24" ht="15.75" customHeight="1">
       <c r="M110" s="122"/>
       <c r="N110" s="1"/>
       <c r="O110" s="24"/>
@@ -9869,7 +9887,7 @@
       <c r="W110" s="17"/>
       <c r="X110" s="1"/>
     </row>
-    <row r="111" spans="8:24" ht="15.75" customHeight="1">
+    <row r="111" spans="1:24" ht="15.75" customHeight="1">
       <c r="M111" s="122"/>
       <c r="N111" s="1"/>
       <c r="O111" s="24"/>
@@ -9880,7 +9898,7 @@
       <c r="W111" s="17"/>
       <c r="X111" s="1"/>
     </row>
-    <row r="112" spans="8:24" ht="15.75" customHeight="1">
+    <row r="112" spans="1:24" ht="15.75" customHeight="1">
       <c r="M112" s="122"/>
       <c r="N112" s="1"/>
       <c r="O112" s="24"/>
@@ -13488,15 +13506,16 @@
     <hyperlink ref="E18" r:id="rId16" display="https://www.amazon.com/dp/B0C6XLS3CT?ref_=ppx_hzsearch_conn_dt_b_fed_asin_title_1" xr:uid="{1722CC90-C648-4234-8233-358B532E3D54}"/>
     <hyperlink ref="E19" r:id="rId17" display="https://www.amazon.com/dp/B08TVLYB3Q?ref_=ppx_hzsearch_conn_dt_b_fed_asin_title_1&amp;th=1" xr:uid="{A4E46ED3-3487-4D3E-A5DA-BCA72136E987}"/>
     <hyperlink ref="E36" r:id="rId18" display="https://www.amazon.com/dp/B08PQPJYHX?ref=ppx_yo2ov_dt_b_fed_asin_title" xr:uid="{C57A72A9-40AF-4547-9693-AC015D139A5D}"/>
+    <hyperlink ref="E101" r:id="rId19" display="https://www.amazon.com/gp/product/B0B1V8D36H?smid=A3FZJTJP2FUJVA&amp;psc=1" xr:uid="{B928DAC3-AD15-48CD-9DB3-A8FADFC3338D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId20"/>
   <tableParts count="5">
-    <tablePart r:id="rId20"/>
     <tablePart r:id="rId21"/>
     <tablePart r:id="rId22"/>
     <tablePart r:id="rId23"/>
     <tablePart r:id="rId24"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Strange commit issue with recent purchase form
testing commit. I expect Sentry section to be populated with lidar item
</commit_message>
<xml_diff>
--- a/Ursaworks Inventory & Purchase.xlsx
+++ b/Ursaworks Inventory & Purchase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluya\Documents\GitHub\Ursaworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluya\Documents\reimbursement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3874BCE1-87E2-4F8C-9C88-293448273571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C80152-125D-425F-9292-598F6ACE81B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="580">
   <si>
     <t>FINANCIAL REPORT</t>
   </si>
@@ -2216,15 +2216,6 @@
   </si>
   <si>
     <t>T-Slot Framing Bar: 20 mm x 20 mm x 10000mm</t>
-  </si>
-  <si>
-    <t>Sentry</t>
-  </si>
-  <si>
-    <t>Lidar</t>
-  </si>
-  <si>
-    <t>Amazon.com: WayPonDEV FHL-LD19 360 Degree 2D Lidar Distance Sensor Kit, 10Hz Scan Rate and 12m Distance Lidar Scanner Module for Smart Obstacle/Robot/Maker Education Indoor/Outdoor : Industrial &amp; Scientific</t>
   </si>
 </sst>
 </file>
@@ -6426,7 +6417,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -9707,7 +9698,7 @@
       <c r="W96" s="17"/>
       <c r="X96" s="1"/>
     </row>
-    <row r="97" spans="1:24" ht="15.75" customHeight="1">
+    <row r="97" spans="8:24" ht="15.75" customHeight="1">
       <c r="H97" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9721,7 +9712,7 @@
       <c r="W97" s="17"/>
       <c r="X97" s="1"/>
     </row>
-    <row r="98" spans="1:24" ht="15.75" customHeight="1">
+    <row r="98" spans="8:24" ht="15.75" customHeight="1">
       <c r="H98" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9735,7 +9726,7 @@
       <c r="W98" s="17"/>
       <c r="X98" s="1"/>
     </row>
-    <row r="99" spans="1:24" ht="15.75" customHeight="1">
+    <row r="99" spans="8:24" ht="15.75" customHeight="1">
       <c r="H99" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9749,10 +9740,7 @@
       <c r="W99" s="17"/>
       <c r="X99" s="1"/>
     </row>
-    <row r="100" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A100" t="s">
-        <v>580</v>
-      </c>
+    <row r="100" spans="8:24" ht="15.75" customHeight="1">
       <c r="H100" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9766,13 +9754,7 @@
       <c r="W100" s="17"/>
       <c r="X100" s="1"/>
     </row>
-    <row r="101" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A101" t="s">
-        <v>581</v>
-      </c>
-      <c r="E101" s="116" t="s">
-        <v>582</v>
-      </c>
+    <row r="101" spans="8:24" ht="15.75" customHeight="1">
       <c r="H101" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9786,7 +9768,7 @@
       <c r="W101" s="17"/>
       <c r="X101" s="1"/>
     </row>
-    <row r="102" spans="1:24" ht="15.75" customHeight="1">
+    <row r="102" spans="8:24" ht="15.75" customHeight="1">
       <c r="H102" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9800,7 +9782,7 @@
       <c r="W102" s="17"/>
       <c r="X102" s="1"/>
     </row>
-    <row r="103" spans="1:24" ht="15.75" customHeight="1">
+    <row r="103" spans="8:24" ht="15.75" customHeight="1">
       <c r="H103" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9814,7 +9796,7 @@
       <c r="W103" s="17"/>
       <c r="X103" s="1"/>
     </row>
-    <row r="104" spans="1:24" ht="15.75" customHeight="1">
+    <row r="104" spans="8:24" ht="15.75" customHeight="1">
       <c r="M104" s="122"/>
       <c r="N104" s="1"/>
       <c r="O104" s="24"/>
@@ -9824,7 +9806,7 @@
       <c r="W104" s="17"/>
       <c r="X104" s="1"/>
     </row>
-    <row r="105" spans="1:24" ht="15.75" customHeight="1">
+    <row r="105" spans="8:24" ht="15.75" customHeight="1">
       <c r="M105" s="122"/>
       <c r="N105" s="1"/>
       <c r="O105" s="24"/>
@@ -9834,7 +9816,7 @@
       <c r="W105" s="17"/>
       <c r="X105" s="1"/>
     </row>
-    <row r="106" spans="1:24" ht="15.75" customHeight="1">
+    <row r="106" spans="8:24" ht="15.75" customHeight="1">
       <c r="M106" s="122"/>
       <c r="N106" s="1"/>
       <c r="O106" s="24"/>
@@ -9844,7 +9826,7 @@
       <c r="W106" s="17"/>
       <c r="X106" s="1"/>
     </row>
-    <row r="107" spans="1:24" ht="15.75" customHeight="1">
+    <row r="107" spans="8:24" ht="15.75" customHeight="1">
       <c r="M107" s="122"/>
       <c r="N107" s="1"/>
       <c r="O107" s="24"/>
@@ -9854,7 +9836,7 @@
       <c r="W107" s="17"/>
       <c r="X107" s="1"/>
     </row>
-    <row r="108" spans="1:24" ht="15.75" customHeight="1">
+    <row r="108" spans="8:24" ht="15.75" customHeight="1">
       <c r="M108" s="122"/>
       <c r="N108" s="1"/>
       <c r="O108" s="24"/>
@@ -9865,7 +9847,7 @@
       <c r="W108" s="17"/>
       <c r="X108" s="1"/>
     </row>
-    <row r="109" spans="1:24" ht="15.75" customHeight="1">
+    <row r="109" spans="8:24" ht="15.75" customHeight="1">
       <c r="M109" s="122"/>
       <c r="N109" s="1"/>
       <c r="O109" s="24"/>
@@ -9876,7 +9858,7 @@
       <c r="W109" s="17"/>
       <c r="X109" s="1"/>
     </row>
-    <row r="110" spans="1:24" ht="15.75" customHeight="1">
+    <row r="110" spans="8:24" ht="15.75" customHeight="1">
       <c r="M110" s="122"/>
       <c r="N110" s="1"/>
       <c r="O110" s="24"/>
@@ -9887,7 +9869,7 @@
       <c r="W110" s="17"/>
       <c r="X110" s="1"/>
     </row>
-    <row r="111" spans="1:24" ht="15.75" customHeight="1">
+    <row r="111" spans="8:24" ht="15.75" customHeight="1">
       <c r="M111" s="122"/>
       <c r="N111" s="1"/>
       <c r="O111" s="24"/>
@@ -9898,7 +9880,7 @@
       <c r="W111" s="17"/>
       <c r="X111" s="1"/>
     </row>
-    <row r="112" spans="1:24" ht="15.75" customHeight="1">
+    <row r="112" spans="8:24" ht="15.75" customHeight="1">
       <c r="M112" s="122"/>
       <c r="N112" s="1"/>
       <c r="O112" s="24"/>
@@ -13506,16 +13488,15 @@
     <hyperlink ref="E18" r:id="rId16" display="https://www.amazon.com/dp/B0C6XLS3CT?ref_=ppx_hzsearch_conn_dt_b_fed_asin_title_1" xr:uid="{1722CC90-C648-4234-8233-358B532E3D54}"/>
     <hyperlink ref="E19" r:id="rId17" display="https://www.amazon.com/dp/B08TVLYB3Q?ref_=ppx_hzsearch_conn_dt_b_fed_asin_title_1&amp;th=1" xr:uid="{A4E46ED3-3487-4D3E-A5DA-BCA72136E987}"/>
     <hyperlink ref="E36" r:id="rId18" display="https://www.amazon.com/dp/B08PQPJYHX?ref=ppx_yo2ov_dt_b_fed_asin_title" xr:uid="{C57A72A9-40AF-4547-9693-AC015D139A5D}"/>
-    <hyperlink ref="E101" r:id="rId19" display="https://www.amazon.com/gp/product/B0B1V8D36H?smid=A3FZJTJP2FUJVA&amp;psc=1" xr:uid="{B928DAC3-AD15-48CD-9DB3-A8FADFC3338D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId20"/>
+  <drawing r:id="rId19"/>
   <tableParts count="5">
+    <tablePart r:id="rId20"/>
     <tablePart r:id="rId21"/>
     <tablePart r:id="rId22"/>
     <tablePart r:id="rId23"/>
     <tablePart r:id="rId24"/>
-    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Revert "Strange commit issue with recent purchase form"
This reverts commit b7bfb03b44b4988009aed379d985e96bf3da043d.
</commit_message>
<xml_diff>
--- a/Ursaworks Inventory & Purchase.xlsx
+++ b/Ursaworks Inventory & Purchase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluya\Documents\reimbursement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sluya\Documents\GitHub\Ursaworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C80152-125D-425F-9292-598F6ACE81B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3874BCE1-87E2-4F8C-9C88-293448273571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="583">
   <si>
     <t>FINANCIAL REPORT</t>
   </si>
@@ -2216,6 +2216,15 @@
   </si>
   <si>
     <t>T-Slot Framing Bar: 20 mm x 20 mm x 10000mm</t>
+  </si>
+  <si>
+    <t>Sentry</t>
+  </si>
+  <si>
+    <t>Lidar</t>
+  </si>
+  <si>
+    <t>Amazon.com: WayPonDEV FHL-LD19 360 Degree 2D Lidar Distance Sensor Kit, 10Hz Scan Rate and 12m Distance Lidar Scanner Module for Smart Obstacle/Robot/Maker Education Indoor/Outdoor : Industrial &amp; Scientific</t>
   </si>
 </sst>
 </file>
@@ -6417,7 +6426,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B38" sqref="B38:B39"/>
+      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -9698,7 +9707,7 @@
       <c r="W96" s="17"/>
       <c r="X96" s="1"/>
     </row>
-    <row r="97" spans="8:24" ht="15.75" customHeight="1">
+    <row r="97" spans="1:24" ht="15.75" customHeight="1">
       <c r="H97" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9712,7 +9721,7 @@
       <c r="W97" s="17"/>
       <c r="X97" s="1"/>
     </row>
-    <row r="98" spans="8:24" ht="15.75" customHeight="1">
+    <row r="98" spans="1:24" ht="15.75" customHeight="1">
       <c r="H98" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9726,7 +9735,7 @@
       <c r="W98" s="17"/>
       <c r="X98" s="1"/>
     </row>
-    <row r="99" spans="8:24" ht="15.75" customHeight="1">
+    <row r="99" spans="1:24" ht="15.75" customHeight="1">
       <c r="H99" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9740,7 +9749,10 @@
       <c r="W99" s="17"/>
       <c r="X99" s="1"/>
     </row>
-    <row r="100" spans="8:24" ht="15.75" customHeight="1">
+    <row r="100" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A100" t="s">
+        <v>580</v>
+      </c>
       <c r="H100" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9754,7 +9766,13 @@
       <c r="W100" s="17"/>
       <c r="X100" s="1"/>
     </row>
-    <row r="101" spans="8:24" ht="15.75" customHeight="1">
+    <row r="101" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A101" t="s">
+        <v>581</v>
+      </c>
+      <c r="E101" s="116" t="s">
+        <v>582</v>
+      </c>
       <c r="H101" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9768,7 +9786,7 @@
       <c r="W101" s="17"/>
       <c r="X101" s="1"/>
     </row>
-    <row r="102" spans="8:24" ht="15.75" customHeight="1">
+    <row r="102" spans="1:24" ht="15.75" customHeight="1">
       <c r="H102" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9782,7 +9800,7 @@
       <c r="W102" s="17"/>
       <c r="X102" s="1"/>
     </row>
-    <row r="103" spans="8:24" ht="15.75" customHeight="1">
+    <row r="103" spans="1:24" ht="15.75" customHeight="1">
       <c r="H103" s="123" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -9796,7 +9814,7 @@
       <c r="W103" s="17"/>
       <c r="X103" s="1"/>
     </row>
-    <row r="104" spans="8:24" ht="15.75" customHeight="1">
+    <row r="104" spans="1:24" ht="15.75" customHeight="1">
       <c r="M104" s="122"/>
       <c r="N104" s="1"/>
       <c r="O104" s="24"/>
@@ -9806,7 +9824,7 @@
       <c r="W104" s="17"/>
       <c r="X104" s="1"/>
     </row>
-    <row r="105" spans="8:24" ht="15.75" customHeight="1">
+    <row r="105" spans="1:24" ht="15.75" customHeight="1">
       <c r="M105" s="122"/>
       <c r="N105" s="1"/>
       <c r="O105" s="24"/>
@@ -9816,7 +9834,7 @@
       <c r="W105" s="17"/>
       <c r="X105" s="1"/>
     </row>
-    <row r="106" spans="8:24" ht="15.75" customHeight="1">
+    <row r="106" spans="1:24" ht="15.75" customHeight="1">
       <c r="M106" s="122"/>
       <c r="N106" s="1"/>
       <c r="O106" s="24"/>
@@ -9826,7 +9844,7 @@
       <c r="W106" s="17"/>
       <c r="X106" s="1"/>
     </row>
-    <row r="107" spans="8:24" ht="15.75" customHeight="1">
+    <row r="107" spans="1:24" ht="15.75" customHeight="1">
       <c r="M107" s="122"/>
       <c r="N107" s="1"/>
       <c r="O107" s="24"/>
@@ -9836,7 +9854,7 @@
       <c r="W107" s="17"/>
       <c r="X107" s="1"/>
     </row>
-    <row r="108" spans="8:24" ht="15.75" customHeight="1">
+    <row r="108" spans="1:24" ht="15.75" customHeight="1">
       <c r="M108" s="122"/>
       <c r="N108" s="1"/>
       <c r="O108" s="24"/>
@@ -9847,7 +9865,7 @@
       <c r="W108" s="17"/>
       <c r="X108" s="1"/>
     </row>
-    <row r="109" spans="8:24" ht="15.75" customHeight="1">
+    <row r="109" spans="1:24" ht="15.75" customHeight="1">
       <c r="M109" s="122"/>
       <c r="N109" s="1"/>
       <c r="O109" s="24"/>
@@ -9858,7 +9876,7 @@
       <c r="W109" s="17"/>
       <c r="X109" s="1"/>
     </row>
-    <row r="110" spans="8:24" ht="15.75" customHeight="1">
+    <row r="110" spans="1:24" ht="15.75" customHeight="1">
       <c r="M110" s="122"/>
       <c r="N110" s="1"/>
       <c r="O110" s="24"/>
@@ -9869,7 +9887,7 @@
       <c r="W110" s="17"/>
       <c r="X110" s="1"/>
     </row>
-    <row r="111" spans="8:24" ht="15.75" customHeight="1">
+    <row r="111" spans="1:24" ht="15.75" customHeight="1">
       <c r="M111" s="122"/>
       <c r="N111" s="1"/>
       <c r="O111" s="24"/>
@@ -9880,7 +9898,7 @@
       <c r="W111" s="17"/>
       <c r="X111" s="1"/>
     </row>
-    <row r="112" spans="8:24" ht="15.75" customHeight="1">
+    <row r="112" spans="1:24" ht="15.75" customHeight="1">
       <c r="M112" s="122"/>
       <c r="N112" s="1"/>
       <c r="O112" s="24"/>
@@ -13488,15 +13506,16 @@
     <hyperlink ref="E18" r:id="rId16" display="https://www.amazon.com/dp/B0C6XLS3CT?ref_=ppx_hzsearch_conn_dt_b_fed_asin_title_1" xr:uid="{1722CC90-C648-4234-8233-358B532E3D54}"/>
     <hyperlink ref="E19" r:id="rId17" display="https://www.amazon.com/dp/B08TVLYB3Q?ref_=ppx_hzsearch_conn_dt_b_fed_asin_title_1&amp;th=1" xr:uid="{A4E46ED3-3487-4D3E-A5DA-BCA72136E987}"/>
     <hyperlink ref="E36" r:id="rId18" display="https://www.amazon.com/dp/B08PQPJYHX?ref=ppx_yo2ov_dt_b_fed_asin_title" xr:uid="{C57A72A9-40AF-4547-9693-AC015D139A5D}"/>
+    <hyperlink ref="E101" r:id="rId19" display="https://www.amazon.com/gp/product/B0B1V8D36H?smid=A3FZJTJP2FUJVA&amp;psc=1" xr:uid="{B928DAC3-AD15-48CD-9DB3-A8FADFC3338D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId20"/>
   <tableParts count="5">
-    <tablePart r:id="rId20"/>
     <tablePart r:id="rId21"/>
     <tablePart r:id="rId22"/>
     <tablePart r:id="rId23"/>
     <tablePart r:id="rId24"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>